<commit_message>
Semana 8 - 26/04/2018
</commit_message>
<xml_diff>
--- a/Conocimiento/Metodología/Calculadora (version 1)(1).xlsx
+++ b/Conocimiento/Metodología/Calculadora (version 1)(1).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Descargas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5A8B3DD-9525-4B59-A771-9A0A1CFD758B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6AFDC1-FEC0-42C0-846D-55B2FCD4C628}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12810" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8430" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Costes y presupuesto" sheetId="2" r:id="rId1"/>
@@ -194,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="232" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="221">
   <si>
     <t>Registered time</t>
   </si>
@@ -656,6 +656,207 @@
   </si>
   <si>
     <t>(a partir de marzo)</t>
+  </si>
+  <si>
+    <t>SP S3</t>
+  </si>
+  <si>
+    <t>Boton guardar/publicar</t>
+  </si>
+  <si>
+    <t>Vista solo lectura programador</t>
+  </si>
+  <si>
+    <t>Investigar cifrado</t>
+  </si>
+  <si>
+    <t>Seguridad logica CRUD</t>
+  </si>
+  <si>
+    <t>Persistencia ID Grafica</t>
+  </si>
+  <si>
+    <t>Vista lectura escuela</t>
+  </si>
+  <si>
+    <t>Vista detalle escuela</t>
+  </si>
+  <si>
+    <t>[Analisis]Persistencia ilustraciones</t>
+  </si>
+  <si>
+    <t>[Impl]Persistencia ilustraciones</t>
+  </si>
+  <si>
+    <t>[Analisis]Sandbox</t>
+  </si>
+  <si>
+    <t>[Impl]Sandbox</t>
+  </si>
+  <si>
+    <t>Ejercicio interactivo</t>
+  </si>
+  <si>
+    <t>Tarea periodica cobro</t>
+  </si>
+  <si>
+    <t>Cobro prog paypal</t>
+  </si>
+  <si>
+    <t>Carga inicial datos</t>
+  </si>
+  <si>
+    <t>Creacion video</t>
+  </si>
+  <si>
+    <t>Insercion video</t>
+  </si>
+  <si>
+    <t>Demo semana 1</t>
+  </si>
+  <si>
+    <t>Demo semana 2</t>
+  </si>
+  <si>
+    <t>[Analisis]Librerias excel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Excel tipo </t>
+  </si>
+  <si>
+    <t>Vista excel</t>
+  </si>
+  <si>
+    <t>Tratamiento excel</t>
+  </si>
+  <si>
+    <t>[Analisis]Info segura alumnos</t>
+  </si>
+  <si>
+    <t>[Impl]Info segura</t>
+  </si>
+  <si>
+    <t>Alvaro S</t>
+  </si>
+  <si>
+    <t>Cambio modelo asignaturas</t>
+  </si>
+  <si>
+    <t>Plantilla PDF</t>
+  </si>
+  <si>
+    <t>Escuela gratuita</t>
+  </si>
+  <si>
+    <t>Vigencia licencia</t>
+  </si>
+  <si>
+    <t>Promocionar ejercicio</t>
+  </si>
+  <si>
+    <t>Gestion licencias escuela</t>
+  </si>
+  <si>
+    <t>Cambios modelos (correccion</t>
+  </si>
+  <si>
+    <t>Especificacion req. Y UML</t>
+  </si>
+  <si>
+    <t>Alvaro D</t>
+  </si>
+  <si>
+    <t>Actualizar pantalla ppal</t>
+  </si>
+  <si>
+    <t>Idea video prom</t>
+  </si>
+  <si>
+    <t>Sonido video prom</t>
+  </si>
+  <si>
+    <t>Publicidad RRSS</t>
+  </si>
+  <si>
+    <t>Presentacion Sem1</t>
+  </si>
+  <si>
+    <t>Presentacion Sem2</t>
+  </si>
+  <si>
+    <t>Informe mejora Sem1</t>
+  </si>
+  <si>
+    <t>Informe mejora Sem2</t>
+  </si>
+  <si>
+    <t>Montaje entrega</t>
+  </si>
+  <si>
+    <t>Reuniones pilotaje</t>
+  </si>
+  <si>
+    <t>Plan contingencia</t>
+  </si>
+  <si>
+    <t>Ale G</t>
+  </si>
+  <si>
+    <t>Nav Mejora diseño</t>
+  </si>
+  <si>
+    <t>Navegacion</t>
+  </si>
+  <si>
+    <t>Diseño listados</t>
+  </si>
+  <si>
+    <t>Validacion rojo</t>
+  </si>
+  <si>
+    <t>Mejora diseño notebook</t>
+  </si>
+  <si>
+    <t>Documentacion presupuesto</t>
+  </si>
+  <si>
+    <t>S3 Est.</t>
+  </si>
+  <si>
+    <t>S2 Ded.</t>
+  </si>
+  <si>
+    <t>Diseño y estanradizacion</t>
+  </si>
+  <si>
+    <t>Seguridad Sem 1</t>
+  </si>
+  <si>
+    <t>Seguridad Sem 2</t>
+  </si>
+  <si>
+    <t>Seguridad escuela</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Semana 10</t>
+  </si>
+  <si>
+    <t>Semana 11</t>
+  </si>
+  <si>
+    <t>Semana 12</t>
+  </si>
+  <si>
+    <t>Semana 13</t>
+  </si>
+  <si>
+    <t>Semana 14</t>
+  </si>
+  <si>
+    <t>Semana 15</t>
   </si>
 </sst>
 </file>
@@ -1450,7 +1651,7 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="147">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1553,6 +1754,49 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="47" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="49" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="36" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1580,18 +1824,6 @@
     <xf numFmtId="0" fontId="0" fillId="45" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="44" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="45" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="47" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1601,9 +1833,15 @@
     <xf numFmtId="0" fontId="0" fillId="47" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="50" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="41" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1613,53 +1851,34 @@
     <xf numFmtId="0" fontId="0" fillId="41" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="47" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="45" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="44" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="44" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="49" borderId="21" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="46" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="43" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="13" fillId="47" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="24" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="50" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="13" fillId="43" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="43" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="43" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Énfasis1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -1905,7 +2124,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.4942946623593546</c:v>
+                  <c:v>0.55350965818358699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2957,7 +3176,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>Real 49%</c:v>
+                        <c:v>Real 55%</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -3411,7 +3630,7 @@
                           <c:extLst>
                             <c:ext uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
                             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                              <c16:uniqueId val="{00000000-552C-4BFF-8715-11B02841A290}"/>
+                              <c16:uniqueId val="{00000000-B5E8-4102-A9F2-C6B9F3CE44B9}"/>
                             </c:ext>
                           </c:extLst>
                         </c15:dLbl>
@@ -3584,7 +3803,7 @@
                               <c15:showDataLabelsRange val="1"/>
                             </c:ext>
                             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                              <c16:uniqueId val="{00000001-552C-4BFF-8715-11B02841A290}"/>
+                              <c16:uniqueId val="{00000001-B5E8-4102-A9F2-C6B9F3CE44B9}"/>
                             </c:ext>
                           </c:extLst>
                         </c15:dLbl>
@@ -3803,7 +4022,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.4942946623593546</c:v>
+                  <c:v>0.55350965818358699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4168,7 +4387,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.56999999999999995</c:v>
+                  <c:v>0.8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4226,7 +4445,7 @@
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>0.4942946623593546</c:v>
+                  <c:v>0.55350965818358699</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10755,7 +10974,7 @@
   <dimension ref="A1:P15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10787,12 +11006,12 @@
       <c r="F1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="84" t="s">
+      <c r="J1" s="115" t="s">
         <v>31</v>
       </c>
-      <c r="K1" s="85"/>
-      <c r="L1" s="85"/>
-      <c r="M1" s="86"/>
+      <c r="K1" s="116"/>
+      <c r="L1" s="116"/>
+      <c r="M1" s="117"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="20" t="s">
@@ -11042,8 +11261,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M30"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="M28" sqref="M14:M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11056,21 +11275,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="87" t="s">
+      <c r="A1" s="118" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="87"/>
-      <c r="C1" s="87"/>
-      <c r="D1" s="87"/>
-      <c r="E1" s="87"/>
-      <c r="G1" s="89" t="s">
+      <c r="B1" s="118"/>
+      <c r="C1" s="118"/>
+      <c r="D1" s="118"/>
+      <c r="E1" s="118"/>
+      <c r="G1" s="120" t="s">
         <v>51</v>
       </c>
-      <c r="H1" s="90"/>
-      <c r="J1" s="91" t="s">
+      <c r="H1" s="121"/>
+      <c r="J1" s="122" t="s">
         <v>54</v>
       </c>
-      <c r="K1" s="92"/>
+      <c r="K1" s="123"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="79" t="s">
@@ -11100,9 +11319,8 @@
       <c r="K2" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="62">
-        <f>(E10+K3)/L13</f>
-        <v>0.4942946623593546</v>
+      <c r="M2" s="62" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -11111,7 +11329,7 @@
       </c>
       <c r="B3" s="65">
         <f>SUM('Imputaciones semana'!A$2:A$30)</f>
-        <v>114.6</v>
+        <v>131.6</v>
       </c>
       <c r="C3" s="66">
         <v>27.19</v>
@@ -11122,14 +11340,14 @@
       </c>
       <c r="E3" s="68">
         <f t="shared" ref="E3:E9" si="0">B3*C3</f>
-        <v>3115.9740000000002</v>
+        <v>3578.2040000000002</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" s="62">
         <f>(E10+K3)/L13</f>
-        <v>0.4942946623593546</v>
+        <v>0.55350965818358699</v>
       </c>
       <c r="H3" s="62">
         <v>1</v>
@@ -11148,7 +11366,7 @@
       </c>
       <c r="B4" s="69">
         <f>SUM('Imputaciones semana'!B$2:B$30)</f>
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="C4" s="70">
         <v>11.47</v>
@@ -11159,11 +11377,11 @@
       </c>
       <c r="E4" s="72">
         <f t="shared" si="0"/>
-        <v>1502.5700000000002</v>
+        <v>1743.44</v>
       </c>
       <c r="G4" s="63">
         <f>E10+K3</f>
-        <v>14362.489333333333</v>
+        <v>16083.071833333337</v>
       </c>
       <c r="H4" s="64">
         <v>29000</v>
@@ -11178,18 +11396,18 @@
       </c>
       <c r="B5" s="69">
         <f>SUM('Imputaciones semana'!C$2:C$30)</f>
-        <v>108.5</v>
+        <v>139</v>
       </c>
       <c r="C5" s="70">
         <v>11.47</v>
       </c>
       <c r="D5" s="71">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E5" s="72">
         <f t="shared" si="0"/>
-        <v>1244.4950000000001</v>
+        <v>1594.3300000000002</v>
       </c>
       <c r="G5" t="s">
         <v>56</v>
@@ -11201,21 +11419,21 @@
       </c>
       <c r="B6" s="69">
         <f>SUM('Imputaciones semana'!D$2:D$30)</f>
-        <v>71</v>
+        <v>78.5</v>
       </c>
       <c r="C6" s="70">
         <v>11.47</v>
       </c>
       <c r="D6" s="71">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E6" s="72">
         <f t="shared" si="0"/>
-        <v>814.37</v>
+        <v>900.3950000000001</v>
       </c>
       <c r="G6" s="83">
-        <v>0.56999999999999995</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -11224,7 +11442,7 @@
       </c>
       <c r="B7" s="69">
         <f>SUM('Imputaciones semana'!E$2:E$30)</f>
-        <v>123.5</v>
+        <v>133.5</v>
       </c>
       <c r="C7" s="70">
         <v>16.010000000000002</v>
@@ -11235,7 +11453,7 @@
       </c>
       <c r="E7" s="72">
         <f t="shared" si="0"/>
-        <v>1977.2350000000001</v>
+        <v>2137.335</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -11244,18 +11462,18 @@
       </c>
       <c r="B8" s="69">
         <f>SUM('Imputaciones semana'!F$2:F$30)</f>
-        <v>121.5</v>
+        <v>138.25</v>
       </c>
       <c r="C8" s="70">
         <v>11.47</v>
       </c>
       <c r="D8" s="71">
         <f t="shared" si="1"/>
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E8" s="72">
         <f t="shared" si="0"/>
-        <v>1393.605</v>
+        <v>1585.7275000000002</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -11264,7 +11482,7 @@
       </c>
       <c r="B9" s="73">
         <f>SUM('Imputaciones semana'!G$2:G$30)</f>
-        <v>108.1</v>
+        <v>128.1</v>
       </c>
       <c r="C9" s="74">
         <v>11.47</v>
@@ -11275,33 +11493,36 @@
       </c>
       <c r="E9" s="76">
         <f t="shared" si="0"/>
-        <v>1239.9069999999999</v>
+        <v>1469.307</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10">
         <f>SUM(B3:B9)</f>
-        <v>778.2</v>
+        <v>900.95</v>
+      </c>
+      <c r="C10" s="70">
+        <v>1120</v>
       </c>
       <c r="D10" t="s">
         <v>10</v>
       </c>
       <c r="E10" s="4">
         <f>SUM(E3:E9)</f>
-        <v>11288.155999999999</v>
+        <v>13008.738500000003</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="88" t="s">
+      <c r="A12" s="119" t="s">
         <v>20</v>
       </c>
-      <c r="B12" s="88"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="88"/>
-      <c r="E12" s="88"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="88"/>
-      <c r="H12" s="88"/>
+      <c r="B12" s="119"/>
+      <c r="C12" s="119"/>
+      <c r="D12" s="119"/>
+      <c r="E12" s="119"/>
+      <c r="F12" s="119"/>
+      <c r="G12" s="119"/>
+      <c r="H12" s="119"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
@@ -11383,6 +11604,9 @@
         <f>'Costes y presupuesto'!$F$11/16*K14</f>
         <v>1816.0333333333335</v>
       </c>
+      <c r="M14">
+        <v>2200</v>
+      </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
@@ -11431,6 +11655,9 @@
         <f>'Costes y presupuesto'!$F$11/16*K15</f>
         <v>3632.0666666666671</v>
       </c>
+      <c r="M15">
+        <v>4000</v>
+      </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
@@ -11479,8 +11706,11 @@
         <f>'Costes y presupuesto'!$F$11/16*K16</f>
         <v>5448.1</v>
       </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M16">
+        <v>4600</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>24</v>
       </c>
@@ -11527,8 +11757,11 @@
         <f>'Costes y presupuesto'!$F$11/16*K17</f>
         <v>7264.1333333333341</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>7803</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>25</v>
       </c>
@@ -11575,8 +11808,11 @@
         <f>'Costes y presupuesto'!$F$11/16*K18</f>
         <v>9080.1666666666679</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>26</v>
       </c>
@@ -11623,8 +11859,11 @@
         <f>'Costes y presupuesto'!$F$11/16*K19</f>
         <v>10896.2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>12500</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
         <v>27</v>
       </c>
@@ -11672,42 +11911,45 @@
         <v>12712.233333333335</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="84" t="s">
+        <v>46</v>
+      </c>
       <c r="B21" s="36">
         <f>('Imputaciones semana'!A9)*$C$3</f>
-        <v>0</v>
+        <v>462.23</v>
       </c>
       <c r="C21" s="37">
         <f>('Imputaciones semana'!B9)*$C$4</f>
-        <v>0</v>
+        <v>240.87</v>
       </c>
       <c r="D21" s="37">
         <f>('Imputaciones semana'!C9)*$C$5</f>
-        <v>0</v>
+        <v>349.83500000000004</v>
       </c>
       <c r="E21" s="37">
         <f>('Imputaciones semana'!D9)*$C$6</f>
-        <v>0</v>
+        <v>86.025000000000006</v>
       </c>
       <c r="F21" s="37">
         <f>('Imputaciones semana'!E9)*$C$7</f>
-        <v>0</v>
+        <v>160.10000000000002</v>
       </c>
       <c r="G21" s="37">
         <f>('Imputaciones semana'!F9)*$C$8</f>
-        <v>0</v>
+        <v>192.1225</v>
       </c>
       <c r="H21" s="38">
         <f>('Imputaciones semana'!G9)*$C$9</f>
-        <v>0</v>
+        <v>229.4</v>
       </c>
       <c r="I21" s="43">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1720.5825</v>
       </c>
       <c r="J21" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K21">
         <v>8</v>
@@ -11717,7 +11959,10 @@
         <v>14528.266666666668</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="84" t="s">
+        <v>47</v>
+      </c>
       <c r="B22" s="39">
         <f>('Imputaciones semana'!A10)*$C$3</f>
         <v>0</v>
@@ -11752,7 +11997,7 @@
       </c>
       <c r="J22" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K22">
         <v>9</v>
@@ -11762,7 +12007,10 @@
         <v>16344.300000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="84" t="s">
+        <v>215</v>
+      </c>
       <c r="B23" s="36">
         <f>('Imputaciones semana'!A11)*$C$3</f>
         <v>0</v>
@@ -11797,7 +12045,7 @@
       </c>
       <c r="J23" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K23">
         <v>10</v>
@@ -11807,7 +12055,10 @@
         <v>18160.333333333336</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="84" t="s">
+        <v>216</v>
+      </c>
       <c r="B24" s="39">
         <f>('Imputaciones semana'!A12)*$C$3</f>
         <v>0</v>
@@ -11842,7 +12093,7 @@
       </c>
       <c r="J24" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K24">
         <v>11</v>
@@ -11852,7 +12103,10 @@
         <v>19976.366666666669</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="84" t="s">
+        <v>217</v>
+      </c>
       <c r="B25" s="36">
         <f>('Imputaciones semana'!A13)*$C$3</f>
         <v>0</v>
@@ -11887,7 +12141,7 @@
       </c>
       <c r="J25" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K25">
         <v>12</v>
@@ -11897,7 +12151,10 @@
         <v>21792.400000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="84" t="s">
+        <v>218</v>
+      </c>
       <c r="B26" s="39">
         <f>('Imputaciones semana'!A14)*$C$3</f>
         <v>0</v>
@@ -11932,7 +12189,7 @@
       </c>
       <c r="J26" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K26">
         <v>13</v>
@@ -11942,7 +12199,10 @@
         <v>23608.433333333334</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="84" t="s">
+        <v>219</v>
+      </c>
       <c r="B27" s="36">
         <f>('Imputaciones semana'!A15)*$C$3</f>
         <v>0</v>
@@ -11977,7 +12237,7 @@
       </c>
       <c r="J27" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K27">
         <v>14</v>
@@ -11987,7 +12247,10 @@
         <v>25424.466666666671</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="84" t="s">
+        <v>220</v>
+      </c>
       <c r="B28" s="39">
         <f>('Imputaciones semana'!A16)*$C$3</f>
         <v>0</v>
@@ -12022,7 +12285,7 @@
       </c>
       <c r="J28" s="4">
         <f t="shared" si="3"/>
-        <v>11288.156000000001</v>
+        <v>13008.738500000001</v>
       </c>
       <c r="K28">
         <v>15</v>
@@ -12032,7 +12295,7 @@
         <v>27240.500000000004</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K29">
         <v>16</v>
       </c>
@@ -12041,7 +12304,7 @@
         <v>29056.533333333336</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="6" t="s">
         <v>48</v>
       </c>
@@ -12093,17 +12356,18 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{73161B54-FF6D-4BF5-9258-A64C5BD1513B}">
-  <dimension ref="A1:W51"/>
+  <dimension ref="A1:Z114"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="V20" sqref="V20"/>
+    <sheetView topLeftCell="F1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Z12" sqref="Z12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="20" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.140625" customWidth="1"/>
+    <col min="12" max="12" width="34.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="14" max="15" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="6.5703125" bestFit="1" customWidth="1"/>
@@ -12114,454 +12378,579 @@
     <col min="23" max="23" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A1" s="91" t="s">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="122" t="s">
         <v>77</v>
       </c>
-      <c r="B1" s="95"/>
-      <c r="C1" s="95"/>
-      <c r="D1" s="95"/>
-      <c r="E1" s="95"/>
-      <c r="F1" s="92"/>
-      <c r="H1" s="105" t="s">
+      <c r="B1" s="133"/>
+      <c r="C1" s="133"/>
+      <c r="D1" s="133"/>
+      <c r="E1" s="133"/>
+      <c r="F1" s="123"/>
+      <c r="H1" s="130" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="106"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="108"/>
-      <c r="L1" s="109" t="s">
+      <c r="I1" s="131"/>
+      <c r="J1" s="132"/>
+      <c r="K1" s="91"/>
+      <c r="L1" s="92" t="s">
         <v>81</v>
       </c>
-      <c r="M1" s="110"/>
-      <c r="N1" s="110"/>
-      <c r="O1" s="111"/>
-      <c r="Q1" s="99" t="s">
+      <c r="M1" s="93"/>
+      <c r="N1" s="93"/>
+      <c r="O1" s="94"/>
+      <c r="Q1" s="124" t="s">
         <v>81</v>
       </c>
-      <c r="R1" s="100"/>
-      <c r="S1" s="100"/>
-      <c r="T1" s="100"/>
-      <c r="U1" s="100"/>
-      <c r="V1" s="100"/>
-      <c r="W1" s="101"/>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A2" s="93" t="s">
+      <c r="R1" s="125"/>
+      <c r="S1" s="125"/>
+      <c r="T1" s="125"/>
+      <c r="U1" s="125"/>
+      <c r="V1" s="125"/>
+      <c r="W1" s="126"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="134" t="s">
         <v>78</v>
       </c>
-      <c r="B2" s="113"/>
-      <c r="C2" s="94"/>
-      <c r="D2" s="93" t="s">
+      <c r="B2" s="135"/>
+      <c r="C2" s="136"/>
+      <c r="D2" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="113"/>
-      <c r="F2" s="94"/>
-      <c r="H2" s="117" t="s">
+      <c r="E2" s="135"/>
+      <c r="F2" s="136"/>
+      <c r="H2" s="99" t="s">
         <v>85</v>
       </c>
-      <c r="I2" s="115" t="s">
+      <c r="I2" s="97" t="s">
         <v>83</v>
       </c>
-      <c r="J2" s="115" t="s">
+      <c r="J2" s="97" t="s">
         <v>84</v>
       </c>
-      <c r="L2" s="97" t="s">
+      <c r="L2" s="86" t="s">
         <v>82</v>
       </c>
-      <c r="M2" s="97" t="s">
+      <c r="M2" s="86" t="s">
         <v>85</v>
       </c>
-      <c r="N2" s="97" t="s">
+      <c r="N2" s="86" t="s">
         <v>83</v>
       </c>
-      <c r="O2" s="102" t="s">
+      <c r="O2" s="88" t="s">
         <v>84</v>
       </c>
-      <c r="Q2" s="97" t="s">
+      <c r="Q2" s="142" t="s">
         <v>82</v>
       </c>
-      <c r="R2" s="97" t="s">
+      <c r="R2" s="142" t="s">
         <v>86</v>
       </c>
-      <c r="S2" s="97" t="s">
+      <c r="S2" s="142" t="s">
         <v>87</v>
       </c>
-      <c r="T2" s="121" t="s">
+      <c r="T2" s="143" t="s">
         <v>89</v>
       </c>
-      <c r="U2" s="102" t="s">
+      <c r="U2" s="144" t="s">
         <v>88</v>
       </c>
-      <c r="V2" s="97" t="s">
+      <c r="V2" s="142" t="s">
         <v>83</v>
       </c>
-      <c r="W2" s="102" t="s">
+      <c r="W2" s="144" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A3" s="112" t="s">
+      <c r="X2" s="144" t="s">
+        <v>208</v>
+      </c>
+      <c r="Y2" s="142" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z2" s="144" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="B3" s="112" t="s">
+      <c r="B3" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="C3" s="112" t="s">
+      <c r="C3" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="D3" s="112" t="s">
+      <c r="D3" s="95" t="s">
         <v>85</v>
       </c>
-      <c r="E3" s="112" t="s">
+      <c r="E3" s="95" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="112" t="s">
+      <c r="F3" s="95" t="s">
         <v>84</v>
       </c>
-      <c r="H3" s="118">
+      <c r="H3" s="100">
         <f>_xlfn.STDEV.S(M3:M9)</f>
         <v>4.4986770542121848</v>
       </c>
-      <c r="I3" s="116">
+      <c r="I3" s="98">
         <f>_xlfn.STDEV.P(N3:N9)</f>
         <v>4.5039665058384131</v>
       </c>
-      <c r="J3" s="119"/>
-      <c r="L3" s="98" t="s">
+      <c r="J3" s="101"/>
+      <c r="L3" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="126">
+      <c r="M3" s="107">
         <v>16</v>
       </c>
-      <c r="N3" s="126">
+      <c r="N3" s="107">
         <v>27</v>
       </c>
-      <c r="O3" s="103"/>
-      <c r="Q3" s="98" t="s">
+      <c r="O3" s="89">
+        <f>M59</f>
+        <v>13</v>
+      </c>
+      <c r="Q3" s="87" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="98">
+      <c r="R3" s="87">
         <v>20</v>
       </c>
-      <c r="S3" s="98">
+      <c r="S3" s="87">
         <v>16</v>
       </c>
-      <c r="T3" s="122">
+      <c r="T3" s="103">
         <f>ABS(R3-S3)/S3</f>
         <v>0.25</v>
       </c>
-      <c r="U3" s="98">
+      <c r="U3" s="87">
         <v>27</v>
       </c>
-      <c r="V3" s="35">
+      <c r="V3" s="145">
         <v>17</v>
       </c>
-      <c r="W3" s="122">
+      <c r="W3" s="103">
         <f>ABS(U3-V3)/V3</f>
         <v>0.58823529411764708</v>
       </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A4" s="114">
+      <c r="X3" s="87">
+        <f>O3</f>
+        <v>13</v>
+      </c>
+      <c r="Y3" s="145">
+        <f>'Imputaciones semana'!A9+'Imputaciones semana'!A10</f>
+        <v>17</v>
+      </c>
+      <c r="Z3" s="103">
+        <f>ABS(X3-Y3)/Y3</f>
+        <v>0.23529411764705882</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="96">
         <v>0</v>
       </c>
-      <c r="B4" s="120"/>
-      <c r="C4" s="120"/>
-      <c r="D4" s="120"/>
-      <c r="E4" s="120"/>
-      <c r="F4" s="120"/>
-      <c r="L4" s="103" t="s">
+      <c r="B4" s="102"/>
+      <c r="C4" s="102"/>
+      <c r="D4" s="102"/>
+      <c r="E4" s="102"/>
+      <c r="F4" s="102"/>
+      <c r="L4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="127">
+      <c r="M4" s="108">
         <v>17</v>
       </c>
-      <c r="N4" s="127">
+      <c r="N4" s="108">
         <v>18</v>
       </c>
-      <c r="O4" s="103"/>
-      <c r="Q4" s="103" t="s">
+      <c r="O4" s="89">
+        <f>M94</f>
+        <v>16</v>
+      </c>
+      <c r="Q4" s="89" t="s">
         <v>2</v>
       </c>
-      <c r="R4" s="103">
+      <c r="R4" s="89">
         <v>20</v>
       </c>
-      <c r="S4" s="103">
+      <c r="S4" s="89">
         <v>17</v>
       </c>
-      <c r="T4" s="122">
+      <c r="T4" s="103">
         <f t="shared" ref="T4:T9" si="0">ABS(R4-S4)/S4</f>
         <v>0.17647058823529413</v>
       </c>
-      <c r="U4" s="103">
+      <c r="U4" s="89">
         <v>22</v>
       </c>
-      <c r="V4" s="103">
+      <c r="V4" s="89">
         <v>21.5</v>
       </c>
-      <c r="W4" s="122">
+      <c r="W4" s="103">
         <f t="shared" ref="W4:W9" si="1">ABS(U4-V4)/V4</f>
         <v>2.3255813953488372E-2</v>
       </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L5" s="103" t="s">
+      <c r="X4" s="87">
+        <f t="shared" ref="X4:X8" si="2">O4</f>
+        <v>16</v>
+      </c>
+      <c r="Y4" s="145">
+        <f>'Imputaciones semana'!B9+'Imputaciones semana'!B10</f>
+        <v>21</v>
+      </c>
+      <c r="Z4" s="103">
+        <f t="shared" ref="Z4:Z9" si="3">ABS(X4-Y4)/Y4</f>
+        <v>0.23809523809523808</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="M5" s="127">
+      <c r="M5" s="108">
         <v>18</v>
       </c>
-      <c r="N5" s="127">
+      <c r="N5" s="108">
         <v>27</v>
       </c>
-      <c r="O5" s="103"/>
-      <c r="Q5" s="103" t="s">
+      <c r="O5" s="89">
+        <f>M66</f>
+        <v>21</v>
+      </c>
+      <c r="Q5" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="R5" s="103">
+      <c r="R5" s="89">
         <v>20</v>
       </c>
-      <c r="S5" s="103">
+      <c r="S5" s="89">
         <v>18</v>
       </c>
-      <c r="T5" s="122">
+      <c r="T5" s="103">
         <f t="shared" si="0"/>
         <v>0.1111111111111111</v>
       </c>
-      <c r="U5" s="103">
+      <c r="U5" s="89">
         <v>27</v>
       </c>
-      <c r="V5" s="35">
+      <c r="V5" s="145">
         <v>14.4</v>
       </c>
-      <c r="W5" s="122">
+      <c r="W5" s="103">
         <f t="shared" si="1"/>
         <v>0.875</v>
       </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="L6" s="103" t="s">
+      <c r="X5" s="87">
+        <f t="shared" si="2"/>
+        <v>21</v>
+      </c>
+      <c r="Y5" s="145">
+        <f>'Imputaciones semana'!C9+'Imputaciones semana'!C10</f>
+        <v>30.5</v>
+      </c>
+      <c r="Z5" s="103">
+        <f t="shared" si="3"/>
+        <v>0.31147540983606559</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="L6" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="M6" s="127">
+      <c r="M6" s="108">
         <v>8</v>
       </c>
-      <c r="N6" s="127">
+      <c r="N6" s="108">
         <v>14</v>
       </c>
-      <c r="O6" s="103"/>
-      <c r="Q6" s="103" t="s">
+      <c r="O6" s="89">
+        <f>M114</f>
+        <v>19</v>
+      </c>
+      <c r="Q6" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="R6" s="103">
+      <c r="R6" s="89">
         <v>20</v>
       </c>
-      <c r="S6" s="103">
+      <c r="S6" s="89">
         <v>8</v>
       </c>
-      <c r="T6" s="122">
+      <c r="T6" s="103">
         <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
-      <c r="U6" s="103">
+      <c r="U6" s="89">
         <v>14</v>
       </c>
-      <c r="V6" s="103">
+      <c r="V6" s="89">
         <v>11</v>
       </c>
-      <c r="W6" s="122">
+      <c r="W6" s="103">
         <f t="shared" si="1"/>
         <v>0.27272727272727271</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A7" s="84" t="s">
+      <c r="X6" s="87">
+        <f t="shared" si="2"/>
+        <v>19</v>
+      </c>
+      <c r="Y6" s="145">
+        <f>'Imputaciones semana'!D9+'Imputaciones semana'!D10</f>
+        <v>7.5</v>
+      </c>
+      <c r="Z6" s="103">
+        <f t="shared" si="3"/>
+        <v>1.5333333333333334</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="115" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="85"/>
-      <c r="C7" s="85"/>
-      <c r="D7" s="86"/>
-      <c r="L7" s="103" t="s">
+      <c r="B7" s="116"/>
+      <c r="C7" s="116"/>
+      <c r="D7" s="117"/>
+      <c r="L7" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="M7" s="127">
+      <c r="M7" s="108">
         <v>12</v>
       </c>
-      <c r="N7" s="127">
+      <c r="N7" s="108">
         <v>23</v>
       </c>
-      <c r="O7" s="103"/>
-      <c r="Q7" s="103" t="s">
+      <c r="O7" s="89">
+        <f>M106</f>
+        <v>23</v>
+      </c>
+      <c r="Q7" s="89" t="s">
         <v>43</v>
       </c>
-      <c r="R7" s="103">
+      <c r="R7" s="89">
         <v>20</v>
       </c>
-      <c r="S7" s="103">
+      <c r="S7" s="89">
         <v>12</v>
       </c>
-      <c r="T7" s="122">
+      <c r="T7" s="103">
         <f t="shared" si="0"/>
         <v>0.66666666666666663</v>
       </c>
-      <c r="U7" s="103">
+      <c r="U7" s="89">
         <v>23</v>
       </c>
-      <c r="V7" s="103">
+      <c r="V7" s="89">
         <v>17</v>
       </c>
-      <c r="W7" s="122">
+      <c r="W7" s="103">
         <f t="shared" si="1"/>
         <v>0.35294117647058826</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A8" s="134" t="s">
+      <c r="X7" s="87">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="Y7" s="145">
+        <f>'Imputaciones semana'!E9+'Imputaciones semana'!E10</f>
+        <v>10</v>
+      </c>
+      <c r="Z7" s="103">
+        <f t="shared" si="3"/>
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="127" t="s">
         <v>83</v>
       </c>
-      <c r="B8" s="135"/>
-      <c r="C8" s="135"/>
-      <c r="D8" s="136"/>
-      <c r="L8" s="103" t="s">
+      <c r="B8" s="128"/>
+      <c r="C8" s="128"/>
+      <c r="D8" s="129"/>
+      <c r="L8" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="M8" s="127">
+      <c r="M8" s="108">
         <v>22</v>
       </c>
-      <c r="N8" s="127">
+      <c r="N8" s="108">
         <v>19</v>
       </c>
-      <c r="O8" s="103"/>
-      <c r="Q8" s="103" t="s">
+      <c r="O8" s="89">
+        <f>M85</f>
+        <v>17</v>
+      </c>
+      <c r="Q8" s="89" t="s">
         <v>44</v>
       </c>
-      <c r="R8" s="103">
+      <c r="R8" s="89">
         <v>20</v>
       </c>
-      <c r="S8" s="103">
+      <c r="S8" s="89">
         <v>22</v>
       </c>
-      <c r="T8" s="122">
+      <c r="T8" s="103">
         <f t="shared" si="0"/>
         <v>9.0909090909090912E-2</v>
       </c>
-      <c r="U8" s="103">
+      <c r="U8" s="89">
         <v>19</v>
       </c>
-      <c r="V8" s="103">
+      <c r="V8" s="89">
         <v>30</v>
       </c>
-      <c r="W8" s="122">
+      <c r="W8" s="103">
         <f t="shared" si="1"/>
         <v>0.36666666666666664</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="X8" s="87">
+        <f t="shared" si="2"/>
+        <v>17</v>
+      </c>
+      <c r="Y8" s="145">
+        <f>'Imputaciones semana'!F9+'Imputaciones semana'!F10</f>
+        <v>16.75</v>
+      </c>
+      <c r="Z8" s="103">
+        <f t="shared" si="3"/>
+        <v>1.4925373134328358E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B9" s="123" t="s">
+      <c r="B9" s="104" t="s">
         <v>128</v>
       </c>
       <c r="C9" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D9" s="123" t="s">
+      <c r="D9" s="104" t="s">
         <v>130</v>
       </c>
-      <c r="L9" s="104" t="s">
+      <c r="L9" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="M9" s="128">
+      <c r="M9" s="109">
         <v>17</v>
       </c>
-      <c r="N9" s="128">
+      <c r="N9" s="109">
         <v>19</v>
       </c>
-      <c r="O9" s="104"/>
-      <c r="Q9" s="104" t="s">
+      <c r="O9" s="90">
+        <f>M77</f>
+        <v>26</v>
+      </c>
+      <c r="Q9" s="90" t="s">
         <v>45</v>
       </c>
-      <c r="R9" s="104">
+      <c r="R9" s="90">
         <v>20</v>
       </c>
-      <c r="S9" s="104">
+      <c r="S9" s="90">
         <v>17</v>
       </c>
-      <c r="T9" s="122">
+      <c r="T9" s="103">
         <f t="shared" si="0"/>
         <v>0.17647058823529413</v>
       </c>
-      <c r="U9" s="104">
+      <c r="U9" s="90">
         <v>19</v>
       </c>
-      <c r="V9" s="104">
+      <c r="V9" s="90">
         <v>21</v>
       </c>
-      <c r="W9" s="122">
+      <c r="W9" s="103">
         <f t="shared" si="1"/>
         <v>9.5238095238095233E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A10" s="130">
+      <c r="X9" s="87">
+        <f>O9</f>
+        <v>26</v>
+      </c>
+      <c r="Y9" s="145">
+        <f>'Imputaciones semana'!G9+'Imputaciones semana'!G10</f>
+        <v>20</v>
+      </c>
+      <c r="Z9" s="103">
+        <f t="shared" si="3"/>
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="111">
         <v>3</v>
       </c>
-      <c r="B10" s="133">
+      <c r="B10" s="114">
         <f>COUNTIF(N12:N51,"&gt;3")</f>
         <v>9</v>
       </c>
-      <c r="C10" s="131">
+      <c r="C10" s="112">
         <f>COUNT(N12:N51)</f>
         <v>40</v>
       </c>
-      <c r="D10" s="133">
+      <c r="D10" s="114">
         <f>B10/C10*100</f>
         <v>22.5</v>
       </c>
-      <c r="S10" s="124" t="s">
+      <c r="S10" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="T10" s="125">
+      <c r="T10" s="106">
         <f>AVERAGEA(T3:T9)</f>
         <v>0.42451829216535092</v>
       </c>
-      <c r="V10" s="124" t="s">
+      <c r="V10" s="105" t="s">
         <v>64</v>
       </c>
-      <c r="W10" s="125">
+      <c r="W10" s="106">
         <f>AVERAGEA(W3:W9)</f>
         <v>0.36772347416767975</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A11" s="134" t="s">
+      <c r="Y10" s="105" t="s">
+        <v>64</v>
+      </c>
+      <c r="Z10" s="106">
+        <f>AVERAGEA(Z3:Z9)</f>
+        <v>0.56187478172086058</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="127" t="s">
         <v>85</v>
       </c>
-      <c r="B11" s="135"/>
-      <c r="C11" s="135"/>
-      <c r="D11" s="136"/>
-      <c r="J11" s="109" t="s">
+      <c r="B11" s="128"/>
+      <c r="C11" s="128"/>
+      <c r="D11" s="129"/>
+      <c r="J11" s="92" t="s">
         <v>132</v>
       </c>
-      <c r="L11" s="109" t="s">
+      <c r="L11" s="92" t="s">
         <v>133</v>
       </c>
-      <c r="M11" s="110"/>
-      <c r="N11" s="110"/>
-      <c r="O11" s="111"/>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="M11" s="93"/>
+      <c r="N11" s="93"/>
+      <c r="O11" s="94"/>
+      <c r="Z11" s="104">
+        <f>Z10/2</f>
+        <v>0.28093739086043029</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="123" t="s">
+      <c r="B12" s="104" t="s">
         <v>128</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="D12" s="123" t="s">
+      <c r="D12" s="104" t="s">
         <v>130</v>
       </c>
       <c r="H12" t="s">
@@ -12573,27 +12962,27 @@
       <c r="J12">
         <v>10</v>
       </c>
-      <c r="K12" s="132"/>
+      <c r="K12" s="113"/>
       <c r="L12" s="70" t="s">
         <v>90</v>
       </c>
-      <c r="N12" s="129">
+      <c r="N12" s="110">
         <v>5</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A13" s="130">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="111">
         <v>3</v>
       </c>
-      <c r="B13" s="133">
+      <c r="B13" s="114">
         <f>COUNTIF(J12:J28,"&gt;3")</f>
         <v>9</v>
       </c>
-      <c r="C13" s="131">
+      <c r="C13" s="112">
         <f>COUNT(J12:J28)</f>
         <v>17</v>
       </c>
-      <c r="D13" s="133">
+      <c r="D13" s="114">
         <f>B13/C13*100</f>
         <v>52.941176470588239</v>
       </c>
@@ -12606,11 +12995,17 @@
       <c r="L13" s="70" t="s">
         <v>91</v>
       </c>
-      <c r="N13" s="129">
+      <c r="N13" s="110">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="127" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="128"/>
+      <c r="C14" s="128"/>
+      <c r="D14" s="129"/>
       <c r="H14" t="s">
         <v>148</v>
       </c>
@@ -12623,12 +13018,24 @@
       <c r="L14" s="70" t="s">
         <v>92</v>
       </c>
-      <c r="N14" s="129">
+      <c r="N14" s="110">
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="F15" s="96"/>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B15" s="104" t="s">
+        <v>128</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="D15" s="104" t="s">
+        <v>130</v>
+      </c>
+      <c r="F15" s="85"/>
       <c r="I15" t="s">
         <v>137</v>
       </c>
@@ -12638,11 +13045,26 @@
       <c r="L15" s="70" t="s">
         <v>93</v>
       </c>
-      <c r="N15" s="129">
+      <c r="N15" s="110">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" s="111">
+        <v>3</v>
+      </c>
+      <c r="B16" s="114">
+        <f>COUNTIF(M54:M58,"&gt;3")+COUNTIF(M60:M65,"&gt;3")+COUNTIF(M67:M76,"&gt;3")+COUNTIF(M78:M84,"&gt;3")+COUNTIF(M86:M93,"&gt;3")+COUNTIF(M95:M105,"&gt;3")+COUNTIF(M107:M113,"&gt;3")</f>
+        <v>9</v>
+      </c>
+      <c r="C16" s="112">
+        <f>COUNT(M54:M58)+COUNT(M60:M65)+COUNT(M67:M76)+COUNT(M78:M84)+COUNT(M86:M93)+COUNT(M95:M105)+COUNT(M107:M113)</f>
+        <v>54</v>
+      </c>
+      <c r="D16" s="114">
+        <f>B16/C16*100</f>
+        <v>16.666666666666664</v>
+      </c>
       <c r="I16" t="s">
         <v>138</v>
       </c>
@@ -12652,7 +13074,7 @@
       <c r="L16" s="70" t="s">
         <v>94</v>
       </c>
-      <c r="N16" s="129">
+      <c r="N16" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12666,7 +13088,7 @@
       <c r="L17" s="70" t="s">
         <v>95</v>
       </c>
-      <c r="N17" s="129">
+      <c r="N17" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12680,7 +13102,7 @@
       <c r="L18" s="70" t="s">
         <v>96</v>
       </c>
-      <c r="N18" s="129">
+      <c r="N18" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12697,7 +13119,7 @@
       <c r="L19" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="N19" s="129">
+      <c r="N19" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12711,7 +13133,7 @@
       <c r="L20" s="70" t="s">
         <v>98</v>
       </c>
-      <c r="N20" s="129">
+      <c r="N20" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12725,7 +13147,7 @@
       <c r="L21" s="70" t="s">
         <v>99</v>
       </c>
-      <c r="N21" s="129">
+      <c r="N21" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12742,7 +13164,7 @@
       <c r="L22" s="70" t="s">
         <v>100</v>
       </c>
-      <c r="N22" s="129">
+      <c r="N22" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12756,7 +13178,7 @@
       <c r="L23" s="70" t="s">
         <v>101</v>
       </c>
-      <c r="N23" s="129">
+      <c r="N23" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12773,7 +13195,7 @@
       <c r="L24" s="70" t="s">
         <v>102</v>
       </c>
-      <c r="N24" s="129">
+      <c r="N24" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12787,7 +13209,7 @@
       <c r="L25" s="70" t="s">
         <v>103</v>
       </c>
-      <c r="N25" s="129">
+      <c r="N25" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12804,7 +13226,7 @@
       <c r="L26" s="70" t="s">
         <v>104</v>
       </c>
-      <c r="N26" s="129">
+      <c r="N26" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12821,7 +13243,7 @@
       <c r="L27" s="70" t="s">
         <v>105</v>
       </c>
-      <c r="N27" s="129">
+      <c r="N27" s="110">
         <v>3</v>
       </c>
     </row>
@@ -12835,7 +13257,7 @@
       <c r="L28" s="70" t="s">
         <v>106</v>
       </c>
-      <c r="N28" s="129">
+      <c r="N28" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12843,7 +13265,7 @@
       <c r="L29" s="70" t="s">
         <v>107</v>
       </c>
-      <c r="N29" s="129">
+      <c r="N29" s="110">
         <v>6</v>
       </c>
     </row>
@@ -12851,7 +13273,7 @@
       <c r="L30" s="70" t="s">
         <v>108</v>
       </c>
-      <c r="N30" s="129">
+      <c r="N30" s="110">
         <v>7</v>
       </c>
     </row>
@@ -12859,7 +13281,7 @@
       <c r="L31" s="70" t="s">
         <v>109</v>
       </c>
-      <c r="N31" s="129">
+      <c r="N31" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12867,7 +13289,7 @@
       <c r="L32" s="70" t="s">
         <v>110</v>
       </c>
-      <c r="N32" s="129">
+      <c r="N32" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12875,7 +13297,7 @@
       <c r="L33" s="70" t="s">
         <v>111</v>
       </c>
-      <c r="N33" s="129">
+      <c r="N33" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12883,7 +13305,7 @@
       <c r="L34" s="70" t="s">
         <v>112</v>
       </c>
-      <c r="N34" s="129">
+      <c r="N34" s="110">
         <v>20</v>
       </c>
     </row>
@@ -12891,7 +13313,7 @@
       <c r="L35" s="70" t="s">
         <v>113</v>
       </c>
-      <c r="N35" s="129">
+      <c r="N35" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12899,7 +13321,7 @@
       <c r="L36" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="N36" s="129">
+      <c r="N36" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12907,7 +13329,7 @@
       <c r="L37" s="70" t="s">
         <v>115</v>
       </c>
-      <c r="N37" s="129">
+      <c r="N37" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12915,7 +13337,7 @@
       <c r="L38" s="70" t="s">
         <v>116</v>
       </c>
-      <c r="N38" s="129">
+      <c r="N38" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12923,7 +13345,7 @@
       <c r="L39" s="70" t="s">
         <v>117</v>
       </c>
-      <c r="N39" s="129">
+      <c r="N39" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12931,7 +13353,7 @@
       <c r="L40" s="70" t="s">
         <v>118</v>
       </c>
-      <c r="N40" s="129">
+      <c r="N40" s="110">
         <v>4</v>
       </c>
     </row>
@@ -12939,7 +13361,7 @@
       <c r="L41" s="70" t="s">
         <v>119</v>
       </c>
-      <c r="N41" s="129">
+      <c r="N41" s="110">
         <v>7</v>
       </c>
     </row>
@@ -12947,7 +13369,7 @@
       <c r="L42" s="70" t="s">
         <v>120</v>
       </c>
-      <c r="N42" s="129">
+      <c r="N42" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12955,7 +13377,7 @@
       <c r="L43" s="70" t="s">
         <v>121</v>
       </c>
-      <c r="N43" s="129">
+      <c r="N43" s="110">
         <v>2</v>
       </c>
     </row>
@@ -12963,7 +13385,7 @@
       <c r="L44" s="70" t="s">
         <v>114</v>
       </c>
-      <c r="N44" s="129">
+      <c r="N44" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12971,7 +13393,7 @@
       <c r="L45" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="N45" s="129">
+      <c r="N45" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12979,7 +13401,7 @@
       <c r="L46" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="N46" s="129">
+      <c r="N46" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12987,7 +13409,7 @@
       <c r="L47" s="70" t="s">
         <v>122</v>
       </c>
-      <c r="N47" s="129">
+      <c r="N47" s="110">
         <v>1</v>
       </c>
     </row>
@@ -12995,36 +13417,562 @@
       <c r="L48" s="70" t="s">
         <v>123</v>
       </c>
-      <c r="N48" s="129">
+      <c r="N48" s="110">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="12:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="11:15" x14ac:dyDescent="0.25">
       <c r="L49" s="70" t="s">
         <v>124</v>
       </c>
-      <c r="N49" s="129">
+      <c r="N49" s="110">
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="12:14" x14ac:dyDescent="0.25">
+    <row r="50" spans="11:15" x14ac:dyDescent="0.25">
       <c r="L50" s="70" t="s">
         <v>125</v>
       </c>
-      <c r="N50" s="129">
+      <c r="N50" s="110">
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="12:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="11:15" x14ac:dyDescent="0.25">
       <c r="L51" s="70" t="s">
         <v>126</v>
       </c>
-      <c r="N51" s="129">
+      <c r="N51" s="110">
         <v>1</v>
       </c>
     </row>
+    <row r="53" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L53" s="138" t="s">
+        <v>154</v>
+      </c>
+      <c r="M53" s="93"/>
+      <c r="N53" s="93"/>
+      <c r="O53" s="94"/>
+    </row>
+    <row r="54" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K54" s="139" t="s">
+        <v>147</v>
+      </c>
+      <c r="L54" s="70" t="s">
+        <v>155</v>
+      </c>
+      <c r="M54">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K55" s="137"/>
+      <c r="L55" s="70" t="s">
+        <v>162</v>
+      </c>
+      <c r="M55">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L56" s="70" t="s">
+        <v>163</v>
+      </c>
+      <c r="M56">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="57" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L57" s="70" t="s">
+        <v>156</v>
+      </c>
+      <c r="M57">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L58" s="70" t="s">
+        <v>157</v>
+      </c>
+      <c r="M58">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L59" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M59" s="141">
+        <f>SUM(M54:M58)</f>
+        <v>13</v>
+      </c>
+    </row>
+    <row r="60" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="K60" s="139" t="s">
+        <v>149</v>
+      </c>
+      <c r="L60" s="70" t="s">
+        <v>158</v>
+      </c>
+      <c r="M60">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L61" s="70" t="s">
+        <v>159</v>
+      </c>
+      <c r="M61">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L62" s="70" t="s">
+        <v>160</v>
+      </c>
+      <c r="M62">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L63" s="70" t="s">
+        <v>161</v>
+      </c>
+      <c r="M63">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="64" spans="11:15" x14ac:dyDescent="0.25">
+      <c r="L64" s="70" t="s">
+        <v>164</v>
+      </c>
+      <c r="M64">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="65" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L65" s="70" t="s">
+        <v>165</v>
+      </c>
+      <c r="M65">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="66" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L66" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M66" s="141">
+        <f>SUM(M60:M65)</f>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="67" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K67" s="139" t="s">
+        <v>151</v>
+      </c>
+      <c r="L67" s="70" t="s">
+        <v>166</v>
+      </c>
+      <c r="M67">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="68" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L68" s="70" t="s">
+        <v>167</v>
+      </c>
+      <c r="M68">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="69" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L69" s="70" t="s">
+        <v>168</v>
+      </c>
+      <c r="M69">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="70" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L70" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="M70">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="71" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L71" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="M71">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="72" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L72" s="70" t="s">
+        <v>171</v>
+      </c>
+      <c r="M72">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="73" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L73" s="70" t="s">
+        <v>172</v>
+      </c>
+      <c r="M73">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="74" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L74" s="70" t="s">
+        <v>211</v>
+      </c>
+      <c r="M74">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="75" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L75" s="70" t="s">
+        <v>212</v>
+      </c>
+      <c r="M75">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="76" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L76" s="70" t="s">
+        <v>173</v>
+      </c>
+      <c r="M76">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L77" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M77" s="141">
+        <f>SUM(M67:M76)</f>
+        <v>26</v>
+      </c>
+    </row>
+    <row r="78" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K78" s="139" t="s">
+        <v>150</v>
+      </c>
+      <c r="L78" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="M78">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="79" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L79" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="M79">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="80" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L80" s="70" t="s">
+        <v>176</v>
+      </c>
+      <c r="M80">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="81" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L81" s="70" t="s">
+        <v>177</v>
+      </c>
+      <c r="M81">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="82" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L82" s="70" t="s">
+        <v>178</v>
+      </c>
+      <c r="M82">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="83" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L83" s="70" t="s">
+        <v>213</v>
+      </c>
+      <c r="M83">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L84" s="70" t="s">
+        <v>179</v>
+      </c>
+      <c r="M84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L85" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M85" s="141">
+        <f>SUM(M79:M84)</f>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="86" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K86" s="139" t="s">
+        <v>180</v>
+      </c>
+      <c r="L86" s="70" t="s">
+        <v>181</v>
+      </c>
+      <c r="M86">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="87" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L87" s="70" t="s">
+        <v>182</v>
+      </c>
+      <c r="M87">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="88" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L88" s="70" t="s">
+        <v>183</v>
+      </c>
+      <c r="M88">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="89" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L89" s="70" t="s">
+        <v>184</v>
+      </c>
+      <c r="M89">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="90" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L90" s="70" t="s">
+        <v>185</v>
+      </c>
+      <c r="M90">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="91" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L91" s="70" t="s">
+        <v>186</v>
+      </c>
+      <c r="M91">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L92" s="70" t="s">
+        <v>187</v>
+      </c>
+      <c r="M92">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="93" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L93" s="70" t="s">
+        <v>188</v>
+      </c>
+      <c r="M93">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L94" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M94" s="141">
+        <f>SUM(M86:M93)</f>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="95" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K95" s="139" t="s">
+        <v>189</v>
+      </c>
+      <c r="L95" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="M95">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="96" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L96" s="70" t="s">
+        <v>191</v>
+      </c>
+      <c r="M96">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="97" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L97" s="70" t="s">
+        <v>192</v>
+      </c>
+      <c r="M97">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="98" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L98" s="70" t="s">
+        <v>193</v>
+      </c>
+      <c r="M98">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="99" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L99" s="70" t="s">
+        <v>194</v>
+      </c>
+      <c r="M99">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L100" s="70" t="s">
+        <v>195</v>
+      </c>
+      <c r="M100">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L101" s="70" t="s">
+        <v>196</v>
+      </c>
+      <c r="M101">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="102" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L102" s="70" t="s">
+        <v>197</v>
+      </c>
+      <c r="M102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L103" s="70" t="s">
+        <v>198</v>
+      </c>
+      <c r="M103">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="104" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L104" s="70" t="s">
+        <v>199</v>
+      </c>
+      <c r="M104">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L105" s="70" t="s">
+        <v>200</v>
+      </c>
+      <c r="M105">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="106" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L106" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M106" s="141">
+        <f>SUM(M95:M105)</f>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="107" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K107" s="139" t="s">
+        <v>201</v>
+      </c>
+      <c r="L107" s="70" t="s">
+        <v>202</v>
+      </c>
+      <c r="M107">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L108" s="70" t="s">
+        <v>203</v>
+      </c>
+      <c r="M108">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="109" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L109" s="70" t="s">
+        <v>210</v>
+      </c>
+      <c r="M109">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="110" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L110" s="70" t="s">
+        <v>204</v>
+      </c>
+      <c r="M110">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L111" s="70" t="s">
+        <v>205</v>
+      </c>
+      <c r="M111">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="L112" s="70" t="s">
+        <v>206</v>
+      </c>
+      <c r="M112">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L113" s="70" t="s">
+        <v>207</v>
+      </c>
+      <c r="M113">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="114" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L114" s="140" t="s">
+        <v>10</v>
+      </c>
+      <c r="M114" s="141">
+        <f>SUM(M107:M113)</f>
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
+    <mergeCell ref="A14:D14"/>
     <mergeCell ref="Q1:W1"/>
     <mergeCell ref="A7:D7"/>
     <mergeCell ref="A8:D8"/>
@@ -13044,7 +13992,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13254,22 +14202,22 @@
       <c r="A8" s="35">
         <v>17</v>
       </c>
-      <c r="B8" s="103">
+      <c r="B8" s="89">
         <v>21.5</v>
       </c>
       <c r="C8" s="35">
         <v>14.4</v>
       </c>
-      <c r="D8" s="103">
+      <c r="D8" s="89">
         <v>11</v>
       </c>
-      <c r="E8" s="103">
+      <c r="E8" s="89">
         <v>17</v>
       </c>
-      <c r="F8" s="103">
+      <c r="F8" s="89">
         <v>30</v>
       </c>
-      <c r="G8" s="104">
+      <c r="G8" s="90">
         <v>21</v>
       </c>
       <c r="H8" t="s">
@@ -13277,13 +14225,27 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="35"/>
-      <c r="B9" s="35"/>
-      <c r="C9" s="35"/>
-      <c r="D9" s="35"/>
-      <c r="E9" s="35"/>
-      <c r="F9" s="35"/>
-      <c r="G9" s="35"/>
+      <c r="A9" s="146">
+        <v>17</v>
+      </c>
+      <c r="B9" s="146">
+        <v>21</v>
+      </c>
+      <c r="C9" s="146">
+        <v>30.5</v>
+      </c>
+      <c r="D9" s="146">
+        <v>7.5</v>
+      </c>
+      <c r="E9" s="146">
+        <v>10</v>
+      </c>
+      <c r="F9" s="146">
+        <v>16.75</v>
+      </c>
+      <c r="G9" s="146">
+        <v>20</v>
+      </c>
       <c r="H9" t="s">
         <v>46</v>
       </c>

</xml_diff>